<commit_message>
Added xlsx to gitignore
</commit_message>
<xml_diff>
--- a/Examples.xlsx
+++ b/Examples.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/felix/Dropbox/02_FH/01 Lehre/BA/Skript-Business-Analytics/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8AE0004F-9F7C-2B4A-8C12-5C828F7283A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A23E888-0AEA-0C49-B97D-F7792F6A3F31}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="34400" yWindow="500" windowWidth="34400" windowHeight="28300" activeTab="6" xr2:uid="{C6296A26-AE79-B143-B067-41BC073D48D8}"/>
+    <workbookView xWindow="34400" yWindow="500" windowWidth="34400" windowHeight="28300" activeTab="7" xr2:uid="{C6296A26-AE79-B143-B067-41BC073D48D8}"/>
   </bookViews>
   <sheets>
     <sheet name="bad" sheetId="1" r:id="rId1"/>
@@ -20,6 +20,7 @@
     <sheet name="forloop2" sheetId="5" r:id="rId5"/>
     <sheet name="transactions" sheetId="6" r:id="rId6"/>
     <sheet name="Spaltenvektor" sheetId="7" r:id="rId7"/>
+    <sheet name="numpy" sheetId="8" r:id="rId8"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -42,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="32">
   <si>
     <t>Ergebnis</t>
   </si>
@@ -126,6 +127,18 @@
   </si>
   <si>
     <t>Matrix (zweidimensional)</t>
+  </si>
+  <si>
+    <t>Tag</t>
+  </si>
+  <si>
+    <t>Wichtige Analyse</t>
+  </si>
+  <si>
+    <t>&gt;20</t>
+  </si>
+  <si>
+    <t>dfdf</t>
   </si>
 </sst>
 </file>
@@ -135,7 +148,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.000000"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -154,6 +167,14 @@
     <font>
       <b/>
       <sz val="20"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="24"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -212,7 +233,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -248,6 +269,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -1038,8 +1060,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C5715453-1EED-344B-831D-27807C0ECE3C}">
   <dimension ref="B2:E18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B24" sqref="B24"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H24" sqref="H24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1141,4 +1163,195 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{90069C3F-3DD8-EE47-9082-BE9CB0B0A051}">
+  <dimension ref="B2:G19"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="88" workbookViewId="0">
+      <selection activeCell="K29" sqref="K29"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="2" spans="2:7" ht="31" x14ac:dyDescent="0.35">
+      <c r="B2" s="15" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="5" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B5" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="6" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B6" s="1">
+        <v>1</v>
+      </c>
+      <c r="C6" s="1">
+        <v>22</v>
+      </c>
+      <c r="D6" s="1">
+        <f>IF(C6&gt;20,C6,0)</f>
+        <v>22</v>
+      </c>
+    </row>
+    <row r="7" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B7" s="1">
+        <v>2</v>
+      </c>
+      <c r="C7" s="1">
+        <v>31</v>
+      </c>
+      <c r="D7" s="1">
+        <f t="shared" ref="D7:D17" si="0">IF(C7&gt;20,C7,0)</f>
+        <v>31</v>
+      </c>
+      <c r="G7" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="8" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B8" s="1">
+        <v>3</v>
+      </c>
+      <c r="C8" s="1">
+        <v>34</v>
+      </c>
+      <c r="D8" s="1">
+        <f t="shared" si="0"/>
+        <v>34</v>
+      </c>
+    </row>
+    <row r="9" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B9" s="1">
+        <v>4</v>
+      </c>
+      <c r="C9" s="1">
+        <v>16</v>
+      </c>
+      <c r="D9" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B10" s="1">
+        <v>5</v>
+      </c>
+      <c r="C10" s="1">
+        <v>8</v>
+      </c>
+      <c r="D10" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B11" s="1">
+        <v>6</v>
+      </c>
+      <c r="C11" s="1">
+        <v>23</v>
+      </c>
+      <c r="D11" s="1">
+        <f t="shared" si="0"/>
+        <v>23</v>
+      </c>
+    </row>
+    <row r="12" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B12" s="1">
+        <v>7</v>
+      </c>
+      <c r="C12" s="1">
+        <v>7</v>
+      </c>
+      <c r="D12" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B13" s="1">
+        <v>8</v>
+      </c>
+      <c r="C13" s="1">
+        <v>26</v>
+      </c>
+      <c r="D13" s="1">
+        <f t="shared" si="0"/>
+        <v>26</v>
+      </c>
+    </row>
+    <row r="14" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B14" s="1">
+        <v>9</v>
+      </c>
+      <c r="C14" s="1">
+        <v>45</v>
+      </c>
+      <c r="D14" s="1">
+        <f t="shared" si="0"/>
+        <v>45</v>
+      </c>
+    </row>
+    <row r="15" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B15" s="1">
+        <v>10</v>
+      </c>
+      <c r="C15" s="1">
+        <v>31</v>
+      </c>
+      <c r="D15" s="1">
+        <f t="shared" si="0"/>
+        <v>31</v>
+      </c>
+    </row>
+    <row r="16" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B16" s="1">
+        <v>11</v>
+      </c>
+      <c r="C16" s="1">
+        <v>3</v>
+      </c>
+      <c r="D16" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B17" s="1">
+        <v>12</v>
+      </c>
+      <c r="C17" s="1">
+        <v>35</v>
+      </c>
+      <c r="D17" s="1">
+        <f>IF(C17&gt;20,C17,0)</f>
+        <v>35</v>
+      </c>
+    </row>
+    <row r="19" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B19" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="C19" s="14">
+        <f>+SUM(C6:C17)</f>
+        <v>281</v>
+      </c>
+      <c r="D19" s="14">
+        <f>+SUM(D6:D17)</f>
+        <v>247</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>